<commit_message>
fix for excel import on windows
</commit_message>
<xml_diff>
--- a/import/vendors.xlsx
+++ b/import/vendors.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekti\Grails\CyberVue\cybervue\import\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
-    <sheet name="Vendors" sheetId="1" r:id="rId4"/>
+    <sheet name="Vendors" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>VendorName</t>
   </si>
@@ -40,7 +44,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -60,7 +64,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica"/>
@@ -72,29 +76,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -235,54 +231,51 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -293,26 +286,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -438,7 +490,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -447,7 +499,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -456,7 +508,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -520,8 +572,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -529,7 +581,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -537,7 +589,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -556,7 +608,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -564,7 +616,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -592,7 +644,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -618,7 +670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -644,7 +696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -670,7 +722,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -696,7 +748,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -722,7 +774,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -748,7 +800,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -774,7 +826,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -800,7 +852,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -813,9 +865,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -832,7 +890,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -851,7 +909,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -877,7 +935,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -903,7 +961,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -929,7 +987,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,7 +1013,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -981,7 +1039,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1007,7 +1065,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1033,7 +1091,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1059,7 +1117,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1085,7 +1143,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1098,9 +1156,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1114,7 +1178,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1133,7 +1197,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1163,7 +1227,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,7 +1253,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1215,7 +1279,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1241,7 +1305,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1267,7 +1331,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1293,7 +1357,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1319,7 +1383,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1345,7 +1409,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1371,7 +1435,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1384,282 +1448,274 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G23"/>
+  <dimension ref="A1:IV22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.6" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="19.5703125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6016" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6016" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.3594" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.0625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6016" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6016" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6016" style="1" customWidth="1"/>
-    <col min="8" max="256" width="19.6016" style="1" customWidth="1"/>
+    <col min="1" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="1" customWidth="1"/>
+    <col min="5" max="256" width="19.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="B3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="C3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="D3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="D4" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>